<commit_message>
moving indices correlation OK
</commit_message>
<xml_diff>
--- a/data files/A-share-index.xlsx
+++ b/data files/A-share-index.xlsx
@@ -32,13 +32,13 @@
     <t>Date</t>
   </si>
   <si>
-    <t>沪深300</t>
+    <t>CSI300</t>
   </si>
   <si>
-    <t>中证500</t>
+    <t>ZhongZheng 500</t>
   </si>
   <si>
-    <t>创业板</t>
+    <t>Chuang Ye Ban</t>
   </si>
 </sst>
 </file>
@@ -99,7 +99,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment vertical="top"/>
@@ -120,6 +120,12 @@
       <alignment vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
   </cellXfs>
@@ -436,21 +442,21 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D3119"/>
+  <dimension ref="A1:D3120"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B3095" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="I7" sqref="I7"/>
+      <selection pane="bottomRight" activeCell="E3118" sqref="E3118"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="12.5703125" style="1" customWidth="1"/>
+    <col min="1" max="1" width="13.85546875" style="1" customWidth="1"/>
     <col min="2" max="2" width="10" style="2" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11" style="2" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10" style="2" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15.42578125" style="2" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14" style="2" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
@@ -44091,8 +44097,14 @@
         <v>1855.9863</v>
       </c>
     </row>
-    <row r="3119" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3119" s="3" t="s">
+    <row r="3118" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3118" s="8"/>
+      <c r="B3118" s="9"/>
+      <c r="C3118" s="9"/>
+      <c r="D3118" s="9"/>
+    </row>
+    <row r="3120" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3120" s="3" t="s">
         <v>0</v>
       </c>
     </row>

</xml_diff>